<commit_message>
Making dims from excel. Still needs the check from them.
</commit_message>
<xml_diff>
--- a/input_data/FlowDirection.xlsx
+++ b/input_data/FlowDirection.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28122"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_7D4755BF84DCCE13E97046798E31F45B5A712953" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{70C126E2-A2EC-4766-8138-7C83236F22D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,6 +28,29 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>Production</t>
+  </si>
+  <si>
+    <t>Production of the flow</t>
+  </si>
+  <si>
+    <t>Consumption</t>
+  </si>
+  <si>
+    <t>Consumption of the flow</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -397,12 +420,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>